<commit_message>
start Bonan and balaine test
</commit_message>
<xml_diff>
--- a/src/premium/Config/filtres_5.xlsx
+++ b/src/premium/Config/filtres_5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remyadda/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remyadda/Desktop/AD/Projets/AD_serveur/src/premium/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0A1A992-968A-6C48-89B8-CE81767A9EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D12F962-0B78-D54F-ADCC-E2B0A52FDE9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5200" windowWidth="28040" windowHeight="16520" xr2:uid="{81B5A901-C830-ED4D-8852-1B248C2D9BB1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{81B5A901-C830-ED4D-8852-1B248C2D9BB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DE78B2-A200-5F43-9BE1-DBB9550EE0FE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,7 +479,7 @@
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.6640625" customWidth="1"/>
     <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="56.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="64" bestFit="1" customWidth="1"/>

</xml_diff>